<commit_message>
/ ‘Thesis/Images/Ti-6246/Microstructures/Edited/Ti6246-1.1.1-CS (500x) - Threshold.xlsx’
</commit_message>
<xml_diff>
--- a/Thesis/Images/Ti-6246/Microstructures/Edited/Ti6246-1.1.1-CS (500x) - Threshold.xlsx
+++ b/Thesis/Images/Ti-6246/Microstructures/Edited/Ti6246-1.1.1-CS (500x) - Threshold.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Solidity</t>
+  </si>
+  <si>
+    <t>Area - 145.73 * 107.25</t>
   </si>
 </sst>
 </file>
@@ -898,9 +901,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M457"/>
+  <dimension ref="A1:P457"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A436" workbookViewId="0">
+      <selection activeCell="Q443" sqref="Q443"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -18616,7 +18621,7 @@
         <v>0.56699999999999995</v>
       </c>
     </row>
-    <row r="433" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>432</v>
       </c>
@@ -18657,7 +18662,7 @@
         <v>0.76600000000000001</v>
       </c>
     </row>
-    <row r="434" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>433</v>
       </c>
@@ -18698,7 +18703,7 @@
         <v>0.45200000000000001</v>
       </c>
     </row>
-    <row r="435" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>434</v>
       </c>
@@ -18739,7 +18744,7 @@
         <v>0.60299999999999998</v>
       </c>
     </row>
-    <row r="436" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>435</v>
       </c>
@@ -18780,7 +18785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="437" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>436</v>
       </c>
@@ -18821,7 +18826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="438" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>437</v>
       </c>
@@ -18861,8 +18866,11 @@
       <c r="M438">
         <v>0.67300000000000004</v>
       </c>
-    </row>
-    <row r="439" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P438" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="439" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>438</v>
       </c>
@@ -18903,7 +18911,7 @@
         <v>0.88900000000000001</v>
       </c>
     </row>
-    <row r="440" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>439</v>
       </c>
@@ -18944,7 +18952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="441" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>440</v>
       </c>
@@ -18985,7 +18993,7 @@
         <v>0.83199999999999996</v>
       </c>
     </row>
-    <row r="442" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>441</v>
       </c>
@@ -19026,7 +19034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="443" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>442</v>
       </c>
@@ -19067,7 +19075,7 @@
         <v>0.93300000000000005</v>
       </c>
     </row>
-    <row r="444" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>443</v>
       </c>
@@ -19108,7 +19116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="445" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>444</v>
       </c>
@@ -19149,7 +19157,7 @@
         <v>0.85699999999999998</v>
       </c>
     </row>
-    <row r="446" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>445</v>
       </c>
@@ -19190,7 +19198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="447" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>446</v>
       </c>
@@ -19231,7 +19239,7 @@
         <v>0.65900000000000003</v>
       </c>
     </row>
-    <row r="448" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>447</v>
       </c>

</xml_diff>